<commit_message>
modification nom antiobiotique en francais
</commit_message>
<xml_diff>
--- a/antibiotics_stability.xlsx
+++ b/antibiotics_stability.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/crabolyoann/Dropbox/Personnel/Design/code_project/AntibioDeal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AB2B6CA-D0A0-4D43-8FFE-1BBE6001BF5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{114D836D-F700-5440-87A6-48AA731C8C49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="760" windowWidth="16100" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="760" windowWidth="23680" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="127">
   <si>
     <t>Molecule</t>
   </si>
@@ -40,24 +40,12 @@
     <t>Reference</t>
   </si>
   <si>
-    <t>amoxicillin</t>
-  </si>
-  <si>
-    <t>amoxicillin + clavulanic acid</t>
-  </si>
-  <si>
-    <t>ampicillin + sulbactam</t>
-  </si>
-  <si>
     <t>aztreonam</t>
   </si>
   <si>
     <t>benzylpenicillin</t>
   </si>
   <si>
-    <t>cefazolin</t>
-  </si>
-  <si>
     <t>cefepime</t>
   </si>
   <si>
@@ -67,9 +55,6 @@
     <t>cefotaxime</t>
   </si>
   <si>
-    <t>cefoxitin</t>
-  </si>
-  <si>
     <t>ceftaroline</t>
   </si>
   <si>
@@ -91,21 +76,9 @@
     <t>cefuroxime</t>
   </si>
   <si>
-    <t>clindamycin</t>
-  </si>
-  <si>
-    <t>cloxacillin</t>
-  </si>
-  <si>
-    <t>colistin</t>
-  </si>
-  <si>
     <t>ertapenem</t>
   </si>
   <si>
-    <t>fosfomycin</t>
-  </si>
-  <si>
     <t>imipenem + cilastatin</t>
   </si>
   <si>
@@ -118,27 +91,9 @@
     <t>meropenem + vaborbactam</t>
   </si>
   <si>
-    <t>oxacillin</t>
-  </si>
-  <si>
-    <t>piperacillin</t>
-  </si>
-  <si>
-    <t>piperacillin + tazobactam</t>
-  </si>
-  <si>
     <t>sulfamethoxazole + trimethoprim</t>
   </si>
   <si>
-    <t>teicoplanin</t>
-  </si>
-  <si>
-    <t>temocillin</t>
-  </si>
-  <si>
-    <t>vancomycin</t>
-  </si>
-  <si>
     <t>NaCl 0.9%</t>
   </si>
   <si>
@@ -160,9 +115,6 @@
     <t>10 mg/mL</t>
   </si>
   <si>
-    <t>50 mg/mL</t>
-  </si>
-  <si>
     <t>10–125 mg/mL</t>
   </si>
   <si>
@@ -250,9 +202,6 @@
     <t>2 h</t>
   </si>
   <si>
-    <t>1 h</t>
-  </si>
-  <si>
     <t>4 h</t>
   </si>
   <si>
@@ -407,6 +356,51 @@
   </si>
   <si>
     <t>[47]</t>
+  </si>
+  <si>
+    <t>amoxicilline</t>
+  </si>
+  <si>
+    <t>amoxicilline + clavulanic acid</t>
+  </si>
+  <si>
+    <t>ampicilline + sulbactam</t>
+  </si>
+  <si>
+    <t>cefazoline</t>
+  </si>
+  <si>
+    <t>cefoxitine</t>
+  </si>
+  <si>
+    <t>clindamycine</t>
+  </si>
+  <si>
+    <t>cloxacilline</t>
+  </si>
+  <si>
+    <t>colistine</t>
+  </si>
+  <si>
+    <t>fosfomycine</t>
+  </si>
+  <si>
+    <t>oxacilline</t>
+  </si>
+  <si>
+    <t>piperacilline</t>
+  </si>
+  <si>
+    <t>piperacilline + tazobactam</t>
+  </si>
+  <si>
+    <t>teicoplanine</t>
+  </si>
+  <si>
+    <t>temocilline</t>
+  </si>
+  <si>
+    <t>vancomycine</t>
   </si>
 </sst>
 </file>
@@ -774,17 +768,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" customWidth="1"/>
-    <col min="3" max="3" width="8.83203125" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" customWidth="1"/>
+    <col min="1" max="1" width="40" customWidth="1"/>
+    <col min="2" max="3" width="18.5" customWidth="1"/>
+    <col min="5" max="5" width="30.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -809,826 +803,809 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>112</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="F2" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>112</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="E3" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="F3" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>113</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="D4" t="s">
-        <v>76</v>
+        <v>60</v>
+      </c>
+      <c r="E4" t="s">
+        <v>67</v>
       </c>
       <c r="F4" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>114</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="E5" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="F5" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="D6" t="s">
-        <v>73</v>
-      </c>
-      <c r="E6" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="F6" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="D7" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="F7" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>115</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="D8" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="F8" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>115</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="D9" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="F9" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="F10" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="D11" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="F11" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="F12" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="D13" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="F13" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="D14" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="F14" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>116</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="D15" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
       <c r="F15" t="s">
-        <v>106</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="D16" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="F16" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="C17" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="D17" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="F17" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="C18" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="D18" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="F18" t="s">
-        <v>108</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C19" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="D19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E19" t="s">
+        <v>69</v>
+      </c>
+      <c r="F19" t="s">
         <v>80</v>
-      </c>
-      <c r="F19" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" t="s">
         <v>41</v>
       </c>
-      <c r="C20" t="s">
-        <v>49</v>
-      </c>
       <c r="D20" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="E20" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="F20" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B21" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="C21" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="D21" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="E21" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="F21" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C22" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="D22" t="s">
+        <v>64</v>
+      </c>
+      <c r="E22" t="s">
+        <v>72</v>
+      </c>
+      <c r="F22" t="s">
         <v>80</v>
-      </c>
-      <c r="E22" t="s">
-        <v>88</v>
-      </c>
-      <c r="F22" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C23" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D23" t="s">
-        <v>81</v>
-      </c>
-      <c r="E23" t="s">
-        <v>89</v>
+        <v>57</v>
       </c>
       <c r="F23" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B24" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="D24" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="F24" t="s">
-        <v>110</v>
+        <v>79</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B25" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D25" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="F25" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B26" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="D26" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="F26" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>22</v>
+        <v>117</v>
       </c>
       <c r="B27" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C27" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D27" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="F27" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>23</v>
+        <v>117</v>
       </c>
       <c r="B28" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="C28" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="D28" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="F28" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>23</v>
+        <v>118</v>
       </c>
       <c r="B29" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="C29" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="D29" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="F29" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>24</v>
+        <v>119</v>
       </c>
       <c r="B30" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="C30" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="D30" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="F30" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B31" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="C31" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="D31" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="F31" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B32" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="C32" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D32" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="F32" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>26</v>
+        <v>120</v>
       </c>
       <c r="B33" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="C33" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="D33" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="F33" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B34" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C34" t="s">
-        <v>58</v>
+        <v>28</v>
       </c>
       <c r="D34" t="s">
+        <v>60</v>
+      </c>
+      <c r="E34" t="s">
         <v>73</v>
       </c>
       <c r="F34" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>20</v>
+      </c>
+      <c r="B35" t="s">
+        <v>26</v>
+      </c>
+      <c r="C35" t="s">
         <v>28</v>
       </c>
-      <c r="B35" t="s">
-        <v>41</v>
-      </c>
-      <c r="C35" t="s">
-        <v>43</v>
-      </c>
       <c r="D35" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="E35" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="F35" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B36" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="C36" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="D36" t="s">
-        <v>75</v>
-      </c>
-      <c r="E36" t="s">
-        <v>90</v>
+        <v>63</v>
       </c>
       <c r="F36" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B37" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="C37" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="D37" t="s">
+        <v>60</v>
+      </c>
+      <c r="F37" t="s">
         <v>80</v>
-      </c>
-      <c r="F37" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B38" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="C38" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="D38" t="s">
-        <v>77</v>
+        <v>58</v>
+      </c>
+      <c r="E38" t="s">
+        <v>74</v>
       </c>
       <c r="F38" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>31</v>
+        <v>121</v>
       </c>
       <c r="B39" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="C39" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="D39" t="s">
-        <v>74</v>
-      </c>
-      <c r="E39" t="s">
-        <v>91</v>
+        <v>61</v>
       </c>
       <c r="F39" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>32</v>
+        <v>122</v>
       </c>
       <c r="B40" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="C40" t="s">
-        <v>68</v>
+        <v>31</v>
       </c>
       <c r="D40" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="F40" t="s">
-        <v>124</v>
+        <v>80</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>33</v>
+        <v>123</v>
       </c>
       <c r="B41" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C41" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="D41" t="s">
-        <v>73</v>
+        <v>57</v>
+      </c>
+      <c r="E41" t="s">
+        <v>75</v>
       </c>
       <c r="F41" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B42" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="C42" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="D42" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="E42" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="F42" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>35</v>
+        <v>124</v>
       </c>
       <c r="B43" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="C43" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="D43" t="s">
-        <v>77</v>
-      </c>
-      <c r="E43" t="s">
-        <v>93</v>
+        <v>55</v>
       </c>
       <c r="F43" t="s">
-        <v>126</v>
+        <v>55</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>36</v>
+        <v>125</v>
       </c>
       <c r="B44" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="C44" t="s">
-        <v>71</v>
+        <v>33</v>
       </c>
       <c r="D44" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="F44" t="s">
-        <v>71</v>
+        <v>110</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>37</v>
+        <v>126</v>
       </c>
       <c r="B45" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C45" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="D45" t="s">
-        <v>73</v>
+        <v>57</v>
+      </c>
+      <c r="E45" t="s">
+        <v>77</v>
       </c>
       <c r="F45" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>38</v>
+        <v>126</v>
       </c>
       <c r="B46" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C46" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="D46" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="E46" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="F46" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>38</v>
-      </c>
-      <c r="B47" t="s">
-        <v>41</v>
-      </c>
-      <c r="C47" t="s">
-        <v>72</v>
-      </c>
-      <c r="D47" t="s">
-        <v>73</v>
-      </c>
-      <c r="E47" t="s">
-        <v>95</v>
-      </c>
-      <c r="F47" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>